<commit_message>
Updated File: Models and added ERD jpeg file.
</commit_message>
<xml_diff>
--- a/ERD_Planning/Models.xlsx
+++ b/ERD_Planning/Models.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jw-mac/unit-2-project/ERD_Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAC5F539-DFD3-C346-B6FB-478B7ABE0EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A94F0A-B937-2940-8C89-40D9A57BA6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21900" yWindow="6760" windowWidth="27640" windowHeight="16940" xr2:uid="{3D9EDC57-4DF1-274A-BD55-E14475D81CBD}"/>
+    <workbookView xWindow="27400" yWindow="3040" windowWidth="23680" windowHeight="20320" xr2:uid="{3D9EDC57-4DF1-274A-BD55-E14475D81CBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -42,15 +42,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Field </t>
-  </si>
-  <si>
-    <t>Review_ID</t>
-  </si>
-  <si>
     <t>Ginos</t>
   </si>
   <si>
@@ -78,24 +69,15 @@
     <t>Julio</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Very Good</t>
   </si>
   <si>
-    <t>Rest_id</t>
-  </si>
-  <si>
     <t>SushiLovers</t>
   </si>
   <si>
     <t>Stars</t>
   </si>
   <si>
-    <t>User_id</t>
-  </si>
-  <si>
     <t>Very Bad</t>
   </si>
   <si>
@@ -112,13 +94,76 @@
   </si>
   <si>
     <t>Wagner</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Zip_Code</t>
+  </si>
+  <si>
+    <t>Luigis</t>
+  </si>
+  <si>
+    <t>Restaurants_categories</t>
+  </si>
+  <si>
+    <t>Restaurant_Id</t>
+  </si>
+  <si>
+    <t>Category_Id</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>Brooklyn</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>123 Main</t>
+  </si>
+  <si>
+    <t>221 Flagler</t>
+  </si>
+  <si>
+    <t>142 Backroad</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>Mexican</t>
+  </si>
+  <si>
+    <t>User_Id</t>
+  </si>
+  <si>
+    <t>Joint Table</t>
+  </si>
+  <si>
+    <t>For future</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Restaurant_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -126,13 +171,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -162,9 +227,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,20 +551,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48950B2A-AD39-8044-8450-7B0CF2578299}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -500,183 +578,306 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="1">
+        <v>11204</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="1">
+        <v>33130</v>
+      </c>
+      <c r="G10" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="1">
+        <v>11204</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="C16" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>1</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1">
-        <v>123</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>2</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>1</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>2</v>
-      </c>
-      <c r="B14" s="1" t="s">
+      <c r="B19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>1</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="1">
-        <v>5</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
-      <c r="E18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>2</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1">
-        <v>2</v>
+      <c r="D19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="1">
+        <v>5</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>2</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
         <v>3</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="1">
+      <c r="B22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="1">
         <v>3</v>
       </c>
-      <c r="D20" s="1">
-        <v>2</v>
-      </c>
-      <c r="E20" s="1">
-        <v>1</v>
-      </c>
+      <c r="D22" s="1">
+        <v>2</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="5"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
+        <v>1</v>
+      </c>
+      <c r="B28" s="7">
+        <v>1</v>
+      </c>
+      <c r="C28" s="7">
+        <v>1</v>
+      </c>
+      <c r="D28" s="5"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="5">
+        <v>2</v>
+      </c>
+      <c r="B29" s="7">
+        <v>3</v>
+      </c>
+      <c r="C29" s="7">
+        <v>1</v>
+      </c>
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="5">
+        <v>3</v>
+      </c>
+      <c r="B30" s="7">
+        <v>2</v>
+      </c>
+      <c r="C30" s="7">
+        <v>2</v>
+      </c>
+      <c r="D30" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated ERD Image file.
</commit_message>
<xml_diff>
--- a/ERD_Planning/Models.xlsx
+++ b/ERD_Planning/Models.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jw-mac/unit-2-project/ERD_Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A94F0A-B937-2940-8C89-40D9A57BA6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226CEB09-C8E9-A74D-A965-66D598F095DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27400" yWindow="3040" windowWidth="23680" windowHeight="20320" xr2:uid="{3D9EDC57-4DF1-274A-BD55-E14475D81CBD}"/>
+    <workbookView xWindow="27460" yWindow="7820" windowWidth="23680" windowHeight="20320" xr2:uid="{3D9EDC57-4DF1-274A-BD55-E14475D81CBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,14 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Ginos</t>
   </si>
   <si>
@@ -75,36 +72,18 @@
     <t>SushiLovers</t>
   </si>
   <si>
-    <t>Stars</t>
-  </si>
-  <si>
     <t>Very Bad</t>
   </si>
   <si>
     <t>So so</t>
   </si>
   <si>
-    <t>First_Name</t>
-  </si>
-  <si>
-    <t>Last_Name</t>
-  </si>
-  <si>
     <t>Lucero</t>
   </si>
   <si>
     <t>Wagner</t>
   </si>
   <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Zip_Code</t>
-  </si>
-  <si>
     <t>Luigis</t>
   </si>
   <si>
@@ -138,25 +117,49 @@
     <t>142 Backroad</t>
   </si>
   <si>
-    <t>Street</t>
-  </si>
-  <si>
     <t>Mexican</t>
   </si>
   <si>
-    <t>User_Id</t>
-  </si>
-  <si>
     <t>Joint Table</t>
   </si>
   <si>
     <t>For future</t>
   </si>
   <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>Restaurant_id</t>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>street</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>zip_code</t>
+  </si>
+  <si>
+    <t>category_id</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>restaurant_id</t>
   </si>
 </sst>
 </file>
@@ -554,7 +557,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -567,7 +570,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -575,7 +578,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -583,7 +586,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -591,7 +594,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -599,12 +602,12 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -612,22 +615,22 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -635,16 +638,16 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F9" s="1">
         <v>11204</v>
@@ -658,16 +661,16 @@
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F10" s="1">
         <v>33130</v>
@@ -681,16 +684,16 @@
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F11" s="1">
         <v>11204</v>
@@ -701,7 +704,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -709,10 +712,10 @@
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -720,10 +723,10 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -731,15 +734,15 @@
         <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -747,16 +750,16 @@
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -764,7 +767,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" s="1">
         <v>5</v>
@@ -781,7 +784,7 @@
         <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C21" s="1">
         <v>1</v>
@@ -798,7 +801,7 @@
         <v>3</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C22" s="1">
         <v>3</v>
@@ -818,14 +821,14 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -833,10 +836,10 @@
         <v>0</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D27" s="5"/>
     </row>

</xml_diff>